<commit_message>
Added a React CheatSheet
I've added a React CheatSheet to help me learn React. I think I am getting the hang of it, and I would like to learn as well how to create good UI interfaces.
</commit_message>
<xml_diff>
--- a/Docker Cheatsheet.xlsx
+++ b/Docker Cheatsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor\My Drive\Cheatsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF65BE8E-516F-4452-BAE5-6F1E916E75EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7975749-03F7-48C8-971C-3B4A8C02318F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="13140" windowHeight="15585" tabRatio="688" xr2:uid="{268831AA-0861-45D3-AD72-2730CA8286D3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="688" activeTab="2" xr2:uid="{268831AA-0861-45D3-AD72-2730CA8286D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Explaining Docker" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="97">
   <si>
     <t>Term</t>
   </si>
@@ -448,6 +448,18 @@
   </si>
   <si>
     <t>This is a lot easier than doing Docker Networks on the command line</t>
+  </si>
+  <si>
+    <t>docker images ls</t>
+  </si>
+  <si>
+    <t>Gets info on the size of docker images</t>
+  </si>
+  <si>
+    <t>RUN pip cache purge</t>
+  </si>
+  <si>
+    <t>Caches the stuff afterwards, helping to reduce file size</t>
   </si>
 </sst>
 </file>
@@ -617,6 +629,20 @@
   </cellStyles>
   <dxfs count="30">
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -640,20 +666,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -822,8 +834,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{22DFCE40-9EF9-4683-92CF-01BA77B10E1A}" name="Table2" displayName="Table2" ref="A1:C14" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
-  <autoFilter ref="A1:C14" xr:uid="{22DFCE40-9EF9-4683-92CF-01BA77B10E1A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{22DFCE40-9EF9-4683-92CF-01BA77B10E1A}" name="Table2" displayName="Table2" ref="A1:C15" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+  <autoFilter ref="A1:C15" xr:uid="{22DFCE40-9EF9-4683-92CF-01BA77B10E1A}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{EE3B227B-57B3-4252-9C6E-FD523E72162D}" name="Command" dataDxfId="22"/>
     <tableColumn id="2" xr3:uid="{D1BBFFA2-5C2C-4629-B07E-6950F73A00DB}" name="What it does" dataDxfId="21"/>
@@ -834,8 +846,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CAADDB11-844F-4275-9B78-5E2B37C102E4}" name="Table3" displayName="Table3" ref="A1:C7" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16">
-  <autoFilter ref="A1:C7" xr:uid="{CAADDB11-844F-4275-9B78-5E2B37C102E4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CAADDB11-844F-4275-9B78-5E2B37C102E4}" name="Table3" displayName="Table3" ref="A1:C8" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16">
+  <autoFilter ref="A1:C8" xr:uid="{CAADDB11-844F-4275-9B78-5E2B37C102E4}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5597131B-AA62-4ECE-A122-B3470566A2F5}" name="Command" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{3FBB2443-52B0-4DB9-AF12-DE0B2CD846F8}" name="What it does" dataDxfId="14"/>
@@ -858,7 +870,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0E96CC78-7705-4B1C-9343-1A4EF08F0B6D}" name="Table5" displayName="Table5" ref="A1:C4" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0E96CC78-7705-4B1C-9343-1A4EF08F0B6D}" name="Table5" displayName="Table5" ref="A1:C4" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A1:C4" xr:uid="{0E96CC78-7705-4B1C-9343-1A4EF08F0B6D}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{2999B6B1-A771-4047-976E-C67BD0B2B2CD}" name="Command"/>
@@ -1169,7 +1181,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -1275,10 +1287,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C4AD2B9-9A3F-4ECA-AF82-F7E5BBC709ED}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1413,6 +1425,14 @@
         <v>79</v>
       </c>
     </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1425,10 +1445,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A617F04-DD14-4BB2-8F45-86A9CFA29989}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1510,6 +1530,14 @@
         <v>58</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1522,8 +1550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{228C7590-A104-4896-A5DE-322D37856E12}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>